<commit_message>
Updated spreadsheet with content instance methods.
</commit_message>
<xml_diff>
--- a/extras/docs/Android_SDK_Coverage.xlsx
+++ b/extras/docs/Android_SDK_Coverage.xlsx
@@ -2380,30 +2380,58 @@
       <c r="B17" t="s" s="5">
         <v>45</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="C17" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s" s="7">
+        <v>40</v>
+      </c>
       <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s" s="7">
+        <v>37</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="K17" t="s" s="7">
+        <v>40</v>
+      </c>
       <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
+      <c r="M17" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="N17" t="s" s="7">
+        <v>40</v>
+      </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
+      <c r="Q17" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="R17" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="S17" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="T17" t="s" s="7">
+        <v>37</v>
+      </c>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="6"/>
+      <c r="Y17" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="Z17" t="s" s="7">
+        <v>40</v>
+      </c>
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
       <c r="AC17" s="6"/>

</xml_diff>

<commit_message>
Updated Excel export of coverage spreadsheet.
</commit_message>
<xml_diff>
--- a/extras/docs/Android_SDK_Coverage.xlsx
+++ b/extras/docs/Android_SDK_Coverage.xlsx
@@ -118,13 +118,13 @@
     <t>accessControlPolicy</t>
   </si>
   <si>
+    <t>Beta</t>
+  </si>
+  <si>
     <t>accessControlPolicyAnnc</t>
   </si>
   <si>
     <t>AE</t>
-  </si>
-  <si>
-    <t>Beta</t>
   </si>
   <si>
     <t>AEAnnc</t>
@@ -414,10 +414,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1932,544 +1932,576 @@
       <c r="B9" t="s" s="5">
         <v>34</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
+      <c r="C9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="L9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="M9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="R9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="S9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="T9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="Z9" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" t="s" s="5">
-        <v>35</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" t="s" s="5">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="D11" t="s" s="7">
-        <v>37</v>
+      <c r="C11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s" s="6">
+        <v>35</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="6"/>
-      <c r="G11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="H11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="N11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="R11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="S11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="T11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="Z11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="R11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="S11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="T11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="Z11" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" t="s" s="5">
         <v>39</v>
       </c>
-      <c r="C13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E13" t="s" s="7">
+      <c r="C13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="F13" t="s" s="7">
+      <c r="F13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="G13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="H13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="I13" t="s" s="7">
+      <c r="G13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="J13" t="s" s="7">
+      <c r="J13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="K13" t="s" s="7">
+      <c r="K13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="L13" t="s" s="7">
+      <c r="L13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="M13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="N13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="R13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="S13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="T13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="U13" t="s" s="7">
+      <c r="M13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="R13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="S13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="T13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="U13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="V13" t="s" s="7">
+      <c r="V13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="W13" t="s" s="7">
+      <c r="W13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="X13" t="s" s="7">
+      <c r="X13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="Y13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="Z13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="AA13" t="s" s="7">
+      <c r="Y13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="Z13" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="AA13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="AB13" t="s" s="7">
+      <c r="AB13" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="6"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" t="s" s="5">
         <v>41</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" t="s" s="5">
         <v>42</v>
       </c>
-      <c r="C15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="F15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="G15" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="H15" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="I15" t="s" s="7">
+      <c r="C15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="I15" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="J15" t="s" s="7">
+      <c r="J15" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="K15" t="s" s="7">
+      <c r="K15" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="L15" t="s" s="7">
+      <c r="L15" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="M15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="N15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="O15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="P15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="Q15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="R15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="S15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="T15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="U15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="V15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="W15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="X15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="Y15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="Z15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="AA15" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="AB15" t="s" s="7">
+      <c r="M15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="N15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="O15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="P15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="Q15" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="R15" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="S15" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="T15" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="U15" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="V15" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="W15" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="X15" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="Y15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="Z15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="AA15" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="AB15" t="s" s="6">
         <v>43</v>
       </c>
       <c r="AC15" s="9"/>
-      <c r="AD15" s="6"/>
+      <c r="AD15" s="7"/>
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" t="s" s="5">
         <v>44</v>
       </c>
-      <c r="C16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="F16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="G16" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="H16" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="I16" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="J16" t="s" s="7">
+      <c r="C16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="G16" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="H16" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="I16" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="J16" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="K16" t="s" s="7">
+      <c r="K16" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="L16" t="s" s="7">
+      <c r="L16" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="M16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="N16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="O16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="P16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="Q16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="R16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="S16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="T16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="U16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="V16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="W16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="X16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="Y16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="Z16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="AA16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="AB16" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="6"/>
+      <c r="M16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="N16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="O16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="P16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="Q16" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="R16" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="S16" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="T16" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="U16" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="V16" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="W16" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="X16" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="Y16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="Z16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="AA16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="AB16" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" t="s" s="5">
         <v>45</v>
       </c>
-      <c r="C17" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s" s="7">
+      <c r="C17" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="H17" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" t="s" s="7">
+      <c r="F17" s="7"/>
+      <c r="G17" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="H17" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="L17" s="6"/>
-      <c r="M17" t="s" s="7">
+      <c r="L17" s="7"/>
+      <c r="M17" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="N17" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="R17" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="S17" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="T17" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="N17" t="s" s="7">
+      <c r="Z17" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="R17" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="S17" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="T17" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="Z17" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="6"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" t="s" s="5">
         <v>46</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" s="2"/>
@@ -2488,318 +2520,318 @@
       <c r="F19" t="s" s="10">
         <v>43</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
     </row>
     <row r="20" ht="15" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" t="s" s="5">
         <v>48</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" t="s" s="5">
         <v>49</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6"/>
-      <c r="AB21" s="6"/>
-      <c r="AC21" s="6"/>
-      <c r="AD21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="7"/>
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" t="s" s="5">
         <v>50</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="6"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
+      <c r="AB22" s="7"/>
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="7"/>
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" t="s" s="5">
         <v>51</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
     </row>
     <row r="24" ht="15" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" t="s" s="5">
         <v>52</v>
       </c>
-      <c r="C24" t="s" s="7">
+      <c r="C24" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="D24" t="s" s="7">
+      <c r="D24" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="E24" t="s" s="7">
+      <c r="E24" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="F24" t="s" s="7">
+      <c r="F24" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" t="s" s="7">
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="R24" t="s" s="7">
+      <c r="R24" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="S24" t="s" s="7">
+      <c r="S24" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="T24" t="s" s="7">
+      <c r="T24" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="6"/>
-      <c r="AD24" s="6"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
     </row>
     <row r="25" ht="15" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" t="s" s="5">
         <v>53</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
-      <c r="AA25" s="6"/>
-      <c r="AB25" s="6"/>
-      <c r="AC25" s="6"/>
-      <c r="AD25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AD25" s="7"/>
     </row>
     <row r="26" ht="15" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" t="s" s="5">
         <v>54</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="6"/>
-      <c r="AB26" s="6"/>
-      <c r="AC26" s="6"/>
-      <c r="AD26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="7"/>
+      <c r="AD26" s="7"/>
     </row>
     <row r="27" ht="15" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" t="s" s="5">
         <v>55</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="6"/>
-      <c r="AA27" s="6"/>
-      <c r="AB27" s="6"/>
-      <c r="AC27" s="6"/>
-      <c r="AD27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7"/>
+      <c r="AC27" s="7"/>
+      <c r="AD27" s="7"/>
     </row>
     <row r="28" ht="15" customHeight="1">
       <c r="A28" s="2"/>
@@ -2899,33 +2931,87 @@
       <c r="C29" t="s" s="10">
         <v>43</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="6"/>
-      <c r="AA29" s="6"/>
-      <c r="AB29" s="6"/>
-      <c r="AC29" s="6"/>
-      <c r="AD29" s="6"/>
+      <c r="D29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="F29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="G29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="H29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="I29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="J29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="K29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="L29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="M29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="N29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="O29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="P29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="Q29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="R29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="S29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="T29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="U29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="V29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="W29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="X29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="Y29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="Z29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AA29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AB29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AC29" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AD29" t="s" s="10">
+        <v>43</v>
+      </c>
     </row>
     <row r="30" ht="15" customHeight="1">
       <c r="A30" s="2"/>
@@ -2935,33 +3021,87 @@
       <c r="C30" t="s" s="10">
         <v>43</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="6"/>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="6"/>
-      <c r="AA30" s="6"/>
-      <c r="AB30" s="6"/>
-      <c r="AC30" s="6"/>
-      <c r="AD30" s="6"/>
+      <c r="D30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="F30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="G30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="H30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="I30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="J30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="K30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="L30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="M30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="N30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="O30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="P30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="Q30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="R30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="S30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="T30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="U30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="V30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="W30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="X30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="Y30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="Z30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AA30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AB30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AC30" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AD30" t="s" s="10">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" ht="15" customHeight="1">
       <c r="A31" s="2"/>
@@ -2971,169 +3111,223 @@
       <c r="C31" t="s" s="10">
         <v>43</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
-      <c r="Y31" s="6"/>
-      <c r="Z31" s="6"/>
-      <c r="AA31" s="6"/>
-      <c r="AB31" s="6"/>
-      <c r="AC31" s="6"/>
-      <c r="AD31" s="6"/>
+      <c r="D31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="F31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="G31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="H31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="I31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="J31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="K31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="L31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="M31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="N31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="O31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="P31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="Q31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="R31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="S31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="T31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="U31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="V31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="W31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="X31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="Y31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="Z31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AA31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AB31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AC31" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AD31" t="s" s="10">
+        <v>43</v>
+      </c>
     </row>
     <row r="32" ht="15" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" t="s" s="5">
         <v>60</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6"/>
-      <c r="AA32" s="6"/>
-      <c r="AB32" s="6"/>
-      <c r="AC32" s="6"/>
-      <c r="AD32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="7"/>
     </row>
     <row r="33" ht="15" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" t="s" s="5">
         <v>61</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="6"/>
-      <c r="AB33" s="6"/>
-      <c r="AC33" s="6"/>
-      <c r="AD33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="7"/>
+      <c r="AD33" s="7"/>
     </row>
     <row r="34" ht="15" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" t="s" s="5">
         <v>62</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="6"/>
-      <c r="AA34" s="6"/>
-      <c r="AB34" s="6"/>
-      <c r="AC34" s="6"/>
-      <c r="AD34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7"/>
     </row>
     <row r="35" ht="15" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" t="s" s="5">
         <v>63</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
-      <c r="S35" s="6"/>
-      <c r="T35" s="6"/>
-      <c r="U35" s="6"/>
-      <c r="V35" s="6"/>
-      <c r="W35" s="6"/>
-      <c r="X35" s="6"/>
-      <c r="Y35" s="6"/>
-      <c r="Z35" s="6"/>
-      <c r="AA35" s="6"/>
-      <c r="AB35" s="6"/>
-      <c r="AC35" s="6"/>
-      <c r="AD35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7"/>
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" s="2"/>
@@ -3320,102 +3514,102 @@
       <c r="B38" t="s" s="5">
         <v>66</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
-      <c r="U38" s="6"/>
-      <c r="V38" s="6"/>
-      <c r="W38" s="6"/>
-      <c r="X38" s="6"/>
-      <c r="Y38" s="6"/>
-      <c r="Z38" s="6"/>
-      <c r="AA38" s="6"/>
-      <c r="AB38" s="6"/>
-      <c r="AC38" s="6"/>
-      <c r="AD38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
     </row>
     <row r="39" ht="15" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" t="s" s="5">
         <v>67</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="6"/>
-      <c r="U39" s="6"/>
-      <c r="V39" s="6"/>
-      <c r="W39" s="6"/>
-      <c r="X39" s="6"/>
-      <c r="Y39" s="6"/>
-      <c r="Z39" s="6"/>
-      <c r="AA39" s="6"/>
-      <c r="AB39" s="6"/>
-      <c r="AC39" s="6"/>
-      <c r="AD39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="7"/>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7"/>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7"/>
+      <c r="AC39" s="7"/>
+      <c r="AD39" s="7"/>
     </row>
     <row r="40" ht="15" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" t="s" s="5">
         <v>68</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="6"/>
-      <c r="U40" s="6"/>
-      <c r="V40" s="6"/>
-      <c r="W40" s="6"/>
-      <c r="X40" s="6"/>
-      <c r="Y40" s="6"/>
-      <c r="Z40" s="6"/>
-      <c r="AA40" s="6"/>
-      <c r="AB40" s="6"/>
-      <c r="AC40" s="6"/>
-      <c r="AD40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="7"/>
+      <c r="AA40" s="7"/>
+      <c r="AB40" s="7"/>
+      <c r="AC40" s="7"/>
+      <c r="AD40" s="7"/>
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="A41" s="2"/>
@@ -3782,34 +3976,34 @@
       <c r="B45" t="s" s="5">
         <v>73</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="6"/>
-      <c r="T45" s="6"/>
-      <c r="U45" s="6"/>
-      <c r="V45" s="6"/>
-      <c r="W45" s="6"/>
-      <c r="X45" s="6"/>
-      <c r="Y45" s="6"/>
-      <c r="Z45" s="6"/>
-      <c r="AA45" s="6"/>
-      <c r="AB45" s="6"/>
-      <c r="AC45" s="6"/>
-      <c r="AD45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
+      <c r="V45" s="7"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="7"/>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7"/>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7"/>
+      <c r="AC45" s="7"/>
+      <c r="AD45" s="7"/>
     </row>
     <row r="46" ht="15" customHeight="1">
       <c r="A46" s="2"/>

</xml_diff>

<commit_message>
Updated coverage spreadsheet with subscriptions.
</commit_message>
<xml_diff>
--- a/extras/docs/Android_SDK_Coverage.xlsx
+++ b/extras/docs/Android_SDK_Coverage.xlsx
@@ -19,7 +19,7 @@
     <t>N/A - Not intended as part of the SDK</t>
   </si>
   <si>
-    <t>Alpha - Partly implemented</t>
+    <t>Alpha - Partly implemented / not working</t>
   </si>
   <si>
     <t>Beta - Implemented but not fully tested</t>
@@ -3976,30 +3976,54 @@
       <c r="B45" t="s" s="5">
         <v>73</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
+      <c r="C45" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="D45" t="s" s="6">
+        <v>35</v>
+      </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
+      <c r="G45" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="H45" t="s" s="6">
+        <v>35</v>
+      </c>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
+      <c r="M45" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="N45" t="s" s="6">
+        <v>35</v>
+      </c>
       <c r="O45" s="7"/>
       <c r="P45" s="7"/>
-      <c r="Q45" s="7"/>
-      <c r="R45" s="7"/>
-      <c r="S45" s="7"/>
-      <c r="T45" s="7"/>
+      <c r="Q45" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="R45" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="S45" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="T45" t="s" s="6">
+        <v>35</v>
+      </c>
       <c r="U45" s="7"/>
       <c r="V45" s="7"/>
       <c r="W45" s="7"/>
       <c r="X45" s="7"/>
-      <c r="Y45" s="7"/>
-      <c r="Z45" s="7"/>
+      <c r="Y45" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="Z45" t="s" s="6">
+        <v>40</v>
+      </c>
       <c r="AA45" s="7"/>
       <c r="AB45" s="7"/>
       <c r="AC45" s="7"/>

</xml_diff>